<commit_message>
Update FuelPrices at 2025-03-19 14:58
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -16,9 +16,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +60,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,12 +443,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>LNBSF00</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>LNBSF00</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -455,14 +458,25 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" t="n">
+        <v>790.4</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>45734</v>
-      </c>
-      <c r="B2" t="n">
-        <v>790.4</v>
       </c>
       <c r="C2" t="n">
         <v>806.651</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>795.08</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>45733</v>
+      </c>
+      <c r="C3" t="n">
+        <v>810.465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-03-19 14:59
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,10 +472,21 @@
       <c r="A3" t="n">
         <v>795.08</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="2" t="n">
         <v>45733</v>
       </c>
       <c r="C3" t="n">
+        <v>810.465</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>792.8440000000001</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>45730</v>
+      </c>
+      <c r="C4" t="n">
         <v>810.465</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-03-20 01:56
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,11 +505,22 @@
       <c r="A6" t="n">
         <v>802.724</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="2" t="n">
         <v>45728</v>
       </c>
       <c r="C6" t="n">
         <v>810.465</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>808.9640000000001</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>45735</v>
+      </c>
+      <c r="C7" t="n">
+        <v>806.651</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-03-21 02:28
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,12 +443,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LNBSF00</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>LNBSF00</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -458,68 +458,79 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="2" t="n">
+        <v>45734</v>
+      </c>
+      <c r="B2" t="n">
         <v>790.4</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>45734</v>
       </c>
       <c r="C2" t="n">
         <v>806.651</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="2" t="n">
+        <v>45733</v>
+      </c>
+      <c r="B3" t="n">
         <v>795.08</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>45733</v>
       </c>
       <c r="C3" t="n">
         <v>810.465</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="2" t="n">
+        <v>45730</v>
+      </c>
+      <c r="B4" t="n">
         <v>792.8440000000001</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>45730</v>
       </c>
       <c r="C4" t="n">
         <v>810.465</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="2" t="n">
+        <v>45729</v>
+      </c>
+      <c r="B5" t="n">
         <v>803.816</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>45729</v>
       </c>
       <c r="C5" t="n">
         <v>810.465</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="2" t="n">
+        <v>45728</v>
+      </c>
+      <c r="B6" t="n">
         <v>802.724</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>45728</v>
       </c>
       <c r="C6" t="n">
         <v>810.465</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="2" t="n">
+        <v>45735</v>
+      </c>
+      <c r="B7" t="n">
         <v>808.9640000000001</v>
       </c>
-      <c r="B7" s="3" t="n">
-        <v>45735</v>
-      </c>
       <c r="C7" t="n">
+        <v>806.651</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
+        <v>45736</v>
+      </c>
+      <c r="B8" t="n">
+        <v>823.3680000000001</v>
+      </c>
+      <c r="C8" t="n">
         <v>806.651</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-03-24 02:48
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>MLBSO00</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -453,85 +453,96 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>MLBSO00</t>
+          <t>Date</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>45734</v>
+      <c r="A2" t="n">
+        <v>806.651</v>
       </c>
       <c r="B2" t="n">
         <v>790.4</v>
       </c>
-      <c r="C2" t="n">
-        <v>806.651</v>
+      <c r="C2" s="2" t="n">
+        <v>45734</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45733</v>
+      <c r="A3" t="n">
+        <v>810.465</v>
       </c>
       <c r="B3" t="n">
         <v>795.08</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="2" t="n">
+        <v>45733</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>810.465</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>45730</v>
       </c>
       <c r="B4" t="n">
         <v>792.8440000000001</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="2" t="n">
+        <v>45730</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>810.465</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>45729</v>
       </c>
       <c r="B5" t="n">
         <v>803.816</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="2" t="n">
+        <v>45729</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>810.465</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>45728</v>
       </c>
       <c r="B6" t="n">
         <v>802.724</v>
       </c>
-      <c r="C6" t="n">
-        <v>810.465</v>
+      <c r="C6" s="2" t="n">
+        <v>45728</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>45735</v>
+      <c r="A7" t="n">
+        <v>806.651</v>
       </c>
       <c r="B7" t="n">
         <v>808.9640000000001</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" s="2" t="n">
+        <v>45735</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>806.651</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="n">
-        <v>45736</v>
       </c>
       <c r="B8" t="n">
         <v>823.3680000000001</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="2" t="n">
+        <v>45736</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
         <v>806.651</v>
+      </c>
+      <c r="B9" t="n">
+        <v>823.9400000000001</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>45737</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-03-28 02:22
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,12 +448,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>LNBSF00</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>LNBSF00</t>
         </is>
       </c>
     </row>
@@ -461,88 +461,99 @@
       <c r="A2" t="n">
         <v>806.651</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="2" t="n">
+        <v>45734</v>
+      </c>
+      <c r="C2" t="n">
         <v>790.4</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>45734</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>810.465</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="2" t="n">
+        <v>45733</v>
+      </c>
+      <c r="C3" t="n">
         <v>795.08</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>45733</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>810.465</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="2" t="n">
+        <v>45730</v>
+      </c>
+      <c r="C4" t="n">
         <v>792.8440000000001</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>45730</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>810.465</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="2" t="n">
+        <v>45729</v>
+      </c>
+      <c r="C5" t="n">
         <v>803.816</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>45729</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>810.465</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="2" t="n">
+        <v>45728</v>
+      </c>
+      <c r="C6" t="n">
         <v>802.724</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>45728</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>806.651</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="2" t="n">
+        <v>45735</v>
+      </c>
+      <c r="C7" t="n">
         <v>808.9640000000001</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>45735</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>806.651</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="2" t="n">
+        <v>45736</v>
+      </c>
+      <c r="C8" t="n">
         <v>823.3680000000001</v>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>45736</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>806.651</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="2" t="n">
+        <v>45737</v>
+      </c>
+      <c r="C9" t="n">
         <v>823.9400000000001</v>
       </c>
-      <c r="C9" s="3" t="n">
-        <v>45737</v>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>45740</v>
+      </c>
+      <c r="C10" t="n">
+        <v>788.6319999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-03-28 02:23
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,11 +549,22 @@
       <c r="A10" t="n">
         <v>806.651</v>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="2" t="n">
         <v>45740</v>
       </c>
       <c r="C10" t="n">
         <v>788.6319999999999</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>45741</v>
+      </c>
+      <c r="C11" t="n">
+        <v>785.928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-03-28 06:08
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,11 +582,22 @@
       <c r="A13" t="n">
         <v>806.651</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="2" t="n">
         <v>45734</v>
       </c>
       <c r="C13" t="n">
         <v>790.4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>45743</v>
+      </c>
+      <c r="C14" t="n">
+        <v>771.1079999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-03-31 07:55
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MLBSO00</t>
+          <t>LNBSF00</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -453,151 +453,162 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>LNBSF00</t>
+          <t>MLBSO00</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>806.651</v>
+        <v>790.4</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>45734</v>
       </c>
       <c r="C2" t="n">
-        <v>790.4</v>
+        <v>806.651</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>810.465</v>
+        <v>795.08</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>45733</v>
       </c>
       <c r="C3" t="n">
-        <v>795.08</v>
+        <v>810.465</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>810.465</v>
+        <v>792.8440000000001</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>45730</v>
       </c>
       <c r="C4" t="n">
-        <v>792.8440000000001</v>
+        <v>810.465</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>810.465</v>
+        <v>803.816</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>45729</v>
       </c>
       <c r="C5" t="n">
-        <v>803.816</v>
+        <v>810.465</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>810.465</v>
+        <v>802.724</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>45728</v>
       </c>
       <c r="C6" t="n">
-        <v>802.724</v>
+        <v>810.465</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>806.651</v>
+        <v>808.9640000000001</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>45735</v>
       </c>
       <c r="C7" t="n">
-        <v>808.9640000000001</v>
+        <v>806.651</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>806.651</v>
+        <v>823.3680000000001</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>45736</v>
       </c>
       <c r="C8" t="n">
-        <v>823.3680000000001</v>
+        <v>806.651</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>806.651</v>
+        <v>823.9400000000001</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>45737</v>
       </c>
       <c r="C9" t="n">
-        <v>823.9400000000001</v>
+        <v>806.651</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>806.651</v>
+        <v>788.6319999999999</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>45740</v>
       </c>
       <c r="C10" t="n">
-        <v>788.6319999999999</v>
+        <v>806.651</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>806.651</v>
+        <v>785.928</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>45741</v>
       </c>
       <c r="C11" t="n">
-        <v>785.928</v>
+        <v>806.651</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>806.651</v>
+        <v>773.9160000000001</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>45742</v>
       </c>
       <c r="C12" t="n">
-        <v>773.9160000000001</v>
+        <v>806.651</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>806.651</v>
+        <v>790.4</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>45734</v>
       </c>
       <c r="C13" t="n">
-        <v>790.4</v>
+        <v>806.651</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>806.651</v>
-      </c>
-      <c r="B14" s="3" t="n">
+        <v>771.1079999999999</v>
+      </c>
+      <c r="B14" s="2" t="n">
         <v>45743</v>
       </c>
       <c r="C14" t="n">
-        <v>771.1079999999999</v>
+        <v>806.651</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>760.188</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>45744</v>
+      </c>
+      <c r="C15" t="n">
+        <v>800.9299999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-04 13:20
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,172 +443,183 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LNBSF00</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>MLBSO00</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>LNBSF00</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="2" t="n">
+        <v>45734</v>
+      </c>
+      <c r="B2" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C2" t="n">
         <v>790.4</v>
       </c>
-      <c r="B2" s="2" t="n">
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45733</v>
+      </c>
+      <c r="B3" t="n">
+        <v>810.465</v>
+      </c>
+      <c r="C3" t="n">
+        <v>795.08</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45730</v>
+      </c>
+      <c r="B4" t="n">
+        <v>810.465</v>
+      </c>
+      <c r="C4" t="n">
+        <v>792.8440000000001</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45729</v>
+      </c>
+      <c r="B5" t="n">
+        <v>810.465</v>
+      </c>
+      <c r="C5" t="n">
+        <v>803.816</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45728</v>
+      </c>
+      <c r="B6" t="n">
+        <v>810.465</v>
+      </c>
+      <c r="C6" t="n">
+        <v>802.724</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45735</v>
+      </c>
+      <c r="B7" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C7" t="n">
+        <v>808.9640000000001</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45736</v>
+      </c>
+      <c r="B8" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C8" t="n">
+        <v>823.3680000000001</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45737</v>
+      </c>
+      <c r="B9" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C9" t="n">
+        <v>823.9400000000001</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45740</v>
+      </c>
+      <c r="B10" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C10" t="n">
+        <v>788.6319999999999</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45741</v>
+      </c>
+      <c r="B11" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C11" t="n">
+        <v>785.928</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45742</v>
+      </c>
+      <c r="B12" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C12" t="n">
+        <v>773.9160000000001</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
         <v>45734</v>
       </c>
-      <c r="C2" t="n">
-        <v>806.651</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>795.08</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>45733</v>
-      </c>
-      <c r="C3" t="n">
-        <v>810.465</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>792.8440000000001</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>45730</v>
-      </c>
-      <c r="C4" t="n">
-        <v>810.465</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>803.816</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>45729</v>
-      </c>
-      <c r="C5" t="n">
-        <v>810.465</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>802.724</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>45728</v>
-      </c>
-      <c r="C6" t="n">
-        <v>810.465</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>808.9640000000001</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>45735</v>
-      </c>
-      <c r="C7" t="n">
-        <v>806.651</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>823.3680000000001</v>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>45736</v>
-      </c>
-      <c r="C8" t="n">
-        <v>806.651</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>823.9400000000001</v>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>45737</v>
-      </c>
-      <c r="C9" t="n">
-        <v>806.651</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>788.6319999999999</v>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>45740</v>
-      </c>
-      <c r="C10" t="n">
-        <v>806.651</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>785.928</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>45741</v>
-      </c>
-      <c r="C11" t="n">
-        <v>806.651</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>773.9160000000001</v>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>45742</v>
-      </c>
-      <c r="C12" t="n">
-        <v>806.651</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
+      <c r="B13" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C13" t="n">
         <v>790.4</v>
       </c>
-      <c r="B13" s="2" t="n">
-        <v>45734</v>
-      </c>
-      <c r="C13" t="n">
-        <v>806.651</v>
-      </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="2" t="n">
+        <v>45743</v>
+      </c>
+      <c r="B14" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C14" t="n">
         <v>771.1079999999999</v>
       </c>
-      <c r="B14" s="2" t="n">
-        <v>45743</v>
-      </c>
-      <c r="C14" t="n">
-        <v>806.651</v>
-      </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" s="2" t="n">
+        <v>45744</v>
+      </c>
+      <c r="B15" t="n">
+        <v>800.9299999999999</v>
+      </c>
+      <c r="C15" t="n">
         <v>760.188</v>
       </c>
-      <c r="B15" s="3" t="n">
-        <v>45744</v>
-      </c>
-      <c r="C15" t="n">
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>45748</v>
+      </c>
+      <c r="B16" t="n">
         <v>800.9299999999999</v>
+      </c>
+      <c r="C16" t="n">
+        <v>749.736</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-04 13:21
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,12 +448,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>LNBSF00</t>
+          <t>MLBSO00</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>MLBSO00</t>
+          <t>LNBSF00</t>
         </is>
       </c>
     </row>
@@ -462,10 +462,10 @@
         <v>45734</v>
       </c>
       <c r="B2" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C2" t="n">
         <v>790.4</v>
-      </c>
-      <c r="C2" t="n">
-        <v>806.651</v>
       </c>
     </row>
     <row r="3">
@@ -473,10 +473,10 @@
         <v>45733</v>
       </c>
       <c r="B3" t="n">
+        <v>810.465</v>
+      </c>
+      <c r="C3" t="n">
         <v>795.08</v>
-      </c>
-      <c r="C3" t="n">
-        <v>810.465</v>
       </c>
     </row>
     <row r="4">
@@ -484,10 +484,10 @@
         <v>45730</v>
       </c>
       <c r="B4" t="n">
+        <v>810.465</v>
+      </c>
+      <c r="C4" t="n">
         <v>792.8440000000001</v>
-      </c>
-      <c r="C4" t="n">
-        <v>810.465</v>
       </c>
     </row>
     <row r="5">
@@ -495,10 +495,10 @@
         <v>45729</v>
       </c>
       <c r="B5" t="n">
+        <v>810.465</v>
+      </c>
+      <c r="C5" t="n">
         <v>803.816</v>
-      </c>
-      <c r="C5" t="n">
-        <v>810.465</v>
       </c>
     </row>
     <row r="6">
@@ -506,10 +506,10 @@
         <v>45728</v>
       </c>
       <c r="B6" t="n">
+        <v>810.465</v>
+      </c>
+      <c r="C6" t="n">
         <v>802.724</v>
-      </c>
-      <c r="C6" t="n">
-        <v>810.465</v>
       </c>
     </row>
     <row r="7">
@@ -517,10 +517,10 @@
         <v>45735</v>
       </c>
       <c r="B7" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C7" t="n">
         <v>808.9640000000001</v>
-      </c>
-      <c r="C7" t="n">
-        <v>806.651</v>
       </c>
     </row>
     <row r="8">
@@ -528,10 +528,10 @@
         <v>45736</v>
       </c>
       <c r="B8" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C8" t="n">
         <v>823.3680000000001</v>
-      </c>
-      <c r="C8" t="n">
-        <v>806.651</v>
       </c>
     </row>
     <row r="9">
@@ -539,10 +539,10 @@
         <v>45737</v>
       </c>
       <c r="B9" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C9" t="n">
         <v>823.9400000000001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>806.651</v>
       </c>
     </row>
     <row r="10">
@@ -550,10 +550,10 @@
         <v>45740</v>
       </c>
       <c r="B10" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C10" t="n">
         <v>788.6319999999999</v>
-      </c>
-      <c r="C10" t="n">
-        <v>806.651</v>
       </c>
     </row>
     <row r="11">
@@ -561,10 +561,10 @@
         <v>45741</v>
       </c>
       <c r="B11" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C11" t="n">
         <v>785.928</v>
-      </c>
-      <c r="C11" t="n">
-        <v>806.651</v>
       </c>
     </row>
     <row r="12">
@@ -572,10 +572,10 @@
         <v>45742</v>
       </c>
       <c r="B12" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C12" t="n">
         <v>773.9160000000001</v>
-      </c>
-      <c r="C12" t="n">
-        <v>806.651</v>
       </c>
     </row>
     <row r="13">
@@ -583,10 +583,10 @@
         <v>45734</v>
       </c>
       <c r="B13" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C13" t="n">
         <v>790.4</v>
-      </c>
-      <c r="C13" t="n">
-        <v>806.651</v>
       </c>
     </row>
     <row r="14">
@@ -594,10 +594,10 @@
         <v>45743</v>
       </c>
       <c r="B14" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="C14" t="n">
         <v>771.1079999999999</v>
-      </c>
-      <c r="C14" t="n">
-        <v>806.651</v>
       </c>
     </row>
     <row r="15">
@@ -605,10 +605,10 @@
         <v>45744</v>
       </c>
       <c r="B15" t="n">
+        <v>800.9299999999999</v>
+      </c>
+      <c r="C15" t="n">
         <v>760.188</v>
-      </c>
-      <c r="C15" t="n">
-        <v>800.9299999999999</v>
       </c>
     </row>
     <row r="16">
@@ -616,21 +616,32 @@
         <v>45748</v>
       </c>
       <c r="B16" t="n">
+        <v>800.9299999999999</v>
+      </c>
+      <c r="C16" t="n">
         <v>749.736</v>
       </c>
-      <c r="C16" t="n">
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>45749</v>
+      </c>
+      <c r="B17" t="n">
         <v>800.9299999999999</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="n">
-        <v>45749</v>
-      </c>
-      <c r="B17" t="n">
+      <c r="C17" t="n">
         <v>764.244</v>
       </c>
-      <c r="C17" t="n">
-        <v>800.9299999999999</v>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>45750</v>
+      </c>
+      <c r="B18" t="n">
+        <v>797.116</v>
+      </c>
+      <c r="C18" t="n">
+        <v>753.74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-07 08:29
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,12 +443,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>MLBSO00</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>MLBSO00</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -458,190 +458,201 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>45734</v>
-      </c>
-      <c r="B2" t="n">
-        <v>806.651</v>
       </c>
       <c r="C2" t="n">
         <v>790.4</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" t="n">
+        <v>810.465</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>45733</v>
-      </c>
-      <c r="B3" t="n">
-        <v>810.465</v>
       </c>
       <c r="C3" t="n">
         <v>795.08</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
+      <c r="A4" t="n">
+        <v>810.465</v>
+      </c>
+      <c r="B4" s="2" t="n">
         <v>45730</v>
-      </c>
-      <c r="B4" t="n">
-        <v>810.465</v>
       </c>
       <c r="C4" t="n">
         <v>792.8440000000001</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
+      <c r="A5" t="n">
+        <v>810.465</v>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>45729</v>
-      </c>
-      <c r="B5" t="n">
-        <v>810.465</v>
       </c>
       <c r="C5" t="n">
         <v>803.816</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
+      <c r="A6" t="n">
+        <v>810.465</v>
+      </c>
+      <c r="B6" s="2" t="n">
         <v>45728</v>
-      </c>
-      <c r="B6" t="n">
-        <v>810.465</v>
       </c>
       <c r="C6" t="n">
         <v>802.724</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
+      <c r="A7" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="B7" s="2" t="n">
         <v>45735</v>
-      </c>
-      <c r="B7" t="n">
-        <v>806.651</v>
       </c>
       <c r="C7" t="n">
         <v>808.9640000000001</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n">
+      <c r="A8" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="B8" s="2" t="n">
         <v>45736</v>
-      </c>
-      <c r="B8" t="n">
-        <v>806.651</v>
       </c>
       <c r="C8" t="n">
         <v>823.3680000000001</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n">
+      <c r="A9" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>45737</v>
-      </c>
-      <c r="B9" t="n">
-        <v>806.651</v>
       </c>
       <c r="C9" t="n">
         <v>823.9400000000001</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n">
+      <c r="A10" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>45740</v>
-      </c>
-      <c r="B10" t="n">
-        <v>806.651</v>
       </c>
       <c r="C10" t="n">
         <v>788.6319999999999</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n">
+      <c r="A11" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="B11" s="2" t="n">
         <v>45741</v>
-      </c>
-      <c r="B11" t="n">
-        <v>806.651</v>
       </c>
       <c r="C11" t="n">
         <v>785.928</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n">
+      <c r="A12" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="B12" s="2" t="n">
         <v>45742</v>
-      </c>
-      <c r="B12" t="n">
-        <v>806.651</v>
       </c>
       <c r="C12" t="n">
         <v>773.9160000000001</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n">
+      <c r="A13" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="B13" s="2" t="n">
         <v>45734</v>
-      </c>
-      <c r="B13" t="n">
-        <v>806.651</v>
       </c>
       <c r="C13" t="n">
         <v>790.4</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n">
+      <c r="A14" t="n">
+        <v>806.651</v>
+      </c>
+      <c r="B14" s="2" t="n">
         <v>45743</v>
-      </c>
-      <c r="B14" t="n">
-        <v>806.651</v>
       </c>
       <c r="C14" t="n">
         <v>771.1079999999999</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="n">
+      <c r="A15" t="n">
+        <v>800.9299999999999</v>
+      </c>
+      <c r="B15" s="2" t="n">
         <v>45744</v>
-      </c>
-      <c r="B15" t="n">
-        <v>800.9299999999999</v>
       </c>
       <c r="C15" t="n">
         <v>760.188</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="n">
+      <c r="A16" t="n">
+        <v>800.9299999999999</v>
+      </c>
+      <c r="B16" s="2" t="n">
         <v>45748</v>
-      </c>
-      <c r="B16" t="n">
-        <v>800.9299999999999</v>
       </c>
       <c r="C16" t="n">
         <v>749.736</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="n">
+      <c r="A17" t="n">
+        <v>800.9299999999999</v>
+      </c>
+      <c r="B17" s="2" t="n">
         <v>45749</v>
-      </c>
-      <c r="B17" t="n">
-        <v>800.9299999999999</v>
       </c>
       <c r="C17" t="n">
         <v>764.244</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="n">
+      <c r="A18" t="n">
+        <v>797.116</v>
+      </c>
+      <c r="B18" s="2" t="n">
         <v>45750</v>
-      </c>
-      <c r="B18" t="n">
-        <v>797.116</v>
       </c>
       <c r="C18" t="n">
         <v>753.74</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>791.395</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>45751</v>
+      </c>
+      <c r="C19" t="n">
+        <v>730.444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-14 02:41
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,211 +448,222 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>LNBSF00</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>LNBSF00</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>806.651</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" t="n">
+        <v>790.4</v>
+      </c>
+      <c r="C2" s="2" t="n">
         <v>45734</v>
-      </c>
-      <c r="C2" t="n">
-        <v>790.4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>810.465</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" t="n">
+        <v>795.08</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <v>45733</v>
-      </c>
-      <c r="C3" t="n">
-        <v>795.08</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>810.465</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" t="n">
+        <v>792.8440000000001</v>
+      </c>
+      <c r="C4" s="2" t="n">
         <v>45730</v>
-      </c>
-      <c r="C4" t="n">
-        <v>792.8440000000001</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>810.465</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" t="n">
+        <v>803.816</v>
+      </c>
+      <c r="C5" s="2" t="n">
         <v>45729</v>
-      </c>
-      <c r="C5" t="n">
-        <v>803.816</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>810.465</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" t="n">
+        <v>802.724</v>
+      </c>
+      <c r="C6" s="2" t="n">
         <v>45728</v>
-      </c>
-      <c r="C6" t="n">
-        <v>802.724</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>806.651</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" t="n">
+        <v>808.9640000000001</v>
+      </c>
+      <c r="C7" s="2" t="n">
         <v>45735</v>
-      </c>
-      <c r="C7" t="n">
-        <v>808.9640000000001</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>806.651</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" t="n">
+        <v>823.3680000000001</v>
+      </c>
+      <c r="C8" s="2" t="n">
         <v>45736</v>
-      </c>
-      <c r="C8" t="n">
-        <v>823.3680000000001</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>806.651</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" t="n">
+        <v>823.9400000000001</v>
+      </c>
+      <c r="C9" s="2" t="n">
         <v>45737</v>
-      </c>
-      <c r="C9" t="n">
-        <v>823.9400000000001</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>806.651</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" t="n">
+        <v>788.6319999999999</v>
+      </c>
+      <c r="C10" s="2" t="n">
         <v>45740</v>
-      </c>
-      <c r="C10" t="n">
-        <v>788.6319999999999</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>806.651</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" t="n">
+        <v>785.928</v>
+      </c>
+      <c r="C11" s="2" t="n">
         <v>45741</v>
-      </c>
-      <c r="C11" t="n">
-        <v>785.928</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>806.651</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" t="n">
+        <v>773.9160000000001</v>
+      </c>
+      <c r="C12" s="2" t="n">
         <v>45742</v>
-      </c>
-      <c r="C12" t="n">
-        <v>773.9160000000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>806.651</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" t="n">
+        <v>790.4</v>
+      </c>
+      <c r="C13" s="2" t="n">
         <v>45734</v>
-      </c>
-      <c r="C13" t="n">
-        <v>790.4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>806.651</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" t="n">
+        <v>771.1079999999999</v>
+      </c>
+      <c r="C14" s="2" t="n">
         <v>45743</v>
-      </c>
-      <c r="C14" t="n">
-        <v>771.1079999999999</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>800.9299999999999</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" t="n">
+        <v>760.188</v>
+      </c>
+      <c r="C15" s="2" t="n">
         <v>45744</v>
-      </c>
-      <c r="C15" t="n">
-        <v>760.188</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>800.9299999999999</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" t="n">
+        <v>749.736</v>
+      </c>
+      <c r="C16" s="2" t="n">
         <v>45748</v>
-      </c>
-      <c r="C16" t="n">
-        <v>749.736</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>800.9299999999999</v>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" t="n">
+        <v>764.244</v>
+      </c>
+      <c r="C17" s="2" t="n">
         <v>45749</v>
-      </c>
-      <c r="C17" t="n">
-        <v>764.244</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>797.116</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" t="n">
+        <v>753.74</v>
+      </c>
+      <c r="C18" s="2" t="n">
         <v>45750</v>
-      </c>
-      <c r="C18" t="n">
-        <v>753.74</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>791.395</v>
       </c>
-      <c r="B19" s="3" t="n">
+      <c r="B19" t="n">
+        <v>730.444</v>
+      </c>
+      <c r="C19" s="2" t="n">
         <v>45751</v>
       </c>
-      <c r="C19" t="n">
-        <v>730.444</v>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>781.86</v>
+      </c>
+      <c r="B20" t="n">
+        <v>679.38</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>45754</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-14 02:42
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -706,8 +706,19 @@
       <c r="B24" t="n">
         <v>690.04</v>
       </c>
-      <c r="C24" s="3" t="n">
+      <c r="C24" s="2" t="n">
         <v>45755</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>776.14</v>
+      </c>
+      <c r="B25" t="n">
+        <v>673.0359999999999</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>45756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-14 03:00
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -739,8 +739,19 @@
       <c r="B27" t="n">
         <v>692.068</v>
       </c>
-      <c r="C27" s="3" t="n">
+      <c r="C27" s="2" t="n">
         <v>45758</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>781.86</v>
+      </c>
+      <c r="B28" t="n">
+        <v>679.38</v>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>45754</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-14 03:01
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -750,8 +750,19 @@
       <c r="B28" t="n">
         <v>679.38</v>
       </c>
-      <c r="C28" s="3" t="n">
+      <c r="C28" s="2" t="n">
         <v>45754</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>770.419</v>
+      </c>
+      <c r="B29" t="n">
+        <v>697.8920000000001</v>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>45757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-14 03:39
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -761,8 +761,19 @@
       <c r="B29" t="n">
         <v>697.8920000000001</v>
       </c>
-      <c r="C29" s="3" t="n">
+      <c r="C29" s="2" t="n">
         <v>45757</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>770.419</v>
+      </c>
+      <c r="B30" t="n">
+        <v>692.068</v>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>45758</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-14 03:55
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -772,7 +772,18 @@
       <c r="B30" t="n">
         <v>692.068</v>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" s="2" t="n">
+        <v>45758</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>770.419</v>
+      </c>
+      <c r="B31" t="n">
+        <v>692.068</v>
+      </c>
+      <c r="C31" s="3" t="n">
         <v>45758</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-14 06:08
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MLBSO00</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -453,338 +453,349 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>MLBSO00</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>806.651</v>
+      <c r="A2" s="2" t="n">
+        <v>45734</v>
       </c>
       <c r="B2" t="n">
         <v>790.4</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>45734</v>
+      <c r="C2" t="n">
+        <v>806.651</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>810.465</v>
+      <c r="A3" s="2" t="n">
+        <v>45733</v>
       </c>
       <c r="B3" t="n">
         <v>795.08</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>45733</v>
+      <c r="C3" t="n">
+        <v>810.465</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>810.465</v>
+      <c r="A4" s="2" t="n">
+        <v>45730</v>
       </c>
       <c r="B4" t="n">
         <v>792.8440000000001</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>45730</v>
+      <c r="C4" t="n">
+        <v>810.465</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>810.465</v>
+      <c r="A5" s="2" t="n">
+        <v>45729</v>
       </c>
       <c r="B5" t="n">
         <v>803.816</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>45729</v>
+      <c r="C5" t="n">
+        <v>810.465</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>810.465</v>
+      <c r="A6" s="2" t="n">
+        <v>45728</v>
       </c>
       <c r="B6" t="n">
         <v>802.724</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>45728</v>
+      <c r="C6" t="n">
+        <v>810.465</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>806.651</v>
+      <c r="A7" s="2" t="n">
+        <v>45735</v>
       </c>
       <c r="B7" t="n">
         <v>808.9640000000001</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>45735</v>
+      <c r="C7" t="n">
+        <v>806.651</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>806.651</v>
+      <c r="A8" s="2" t="n">
+        <v>45736</v>
       </c>
       <c r="B8" t="n">
         <v>823.3680000000001</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>45736</v>
+      <c r="C8" t="n">
+        <v>806.651</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>806.651</v>
+      <c r="A9" s="2" t="n">
+        <v>45737</v>
       </c>
       <c r="B9" t="n">
         <v>823.9400000000001</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>45737</v>
+      <c r="C9" t="n">
+        <v>806.651</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>806.651</v>
+      <c r="A10" s="2" t="n">
+        <v>45740</v>
       </c>
       <c r="B10" t="n">
         <v>788.6319999999999</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>45740</v>
+      <c r="C10" t="n">
+        <v>806.651</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>806.651</v>
+      <c r="A11" s="2" t="n">
+        <v>45741</v>
       </c>
       <c r="B11" t="n">
         <v>785.928</v>
       </c>
-      <c r="C11" s="2" t="n">
-        <v>45741</v>
+      <c r="C11" t="n">
+        <v>806.651</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>806.651</v>
+      <c r="A12" s="2" t="n">
+        <v>45742</v>
       </c>
       <c r="B12" t="n">
         <v>773.9160000000001</v>
       </c>
-      <c r="C12" s="2" t="n">
-        <v>45742</v>
+      <c r="C12" t="n">
+        <v>806.651</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>806.651</v>
+      <c r="A13" s="2" t="n">
+        <v>45734</v>
       </c>
       <c r="B13" t="n">
         <v>790.4</v>
       </c>
-      <c r="C13" s="2" t="n">
-        <v>45734</v>
+      <c r="C13" t="n">
+        <v>806.651</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>806.651</v>
+      <c r="A14" s="2" t="n">
+        <v>45743</v>
       </c>
       <c r="B14" t="n">
         <v>771.1079999999999</v>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>45743</v>
+      <c r="C14" t="n">
+        <v>806.651</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>800.9299999999999</v>
+      <c r="A15" s="2" t="n">
+        <v>45744</v>
       </c>
       <c r="B15" t="n">
         <v>760.188</v>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>45744</v>
+      <c r="C15" t="n">
+        <v>800.9299999999999</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>800.9299999999999</v>
+      <c r="A16" s="2" t="n">
+        <v>45748</v>
       </c>
       <c r="B16" t="n">
         <v>749.736</v>
       </c>
-      <c r="C16" s="2" t="n">
-        <v>45748</v>
+      <c r="C16" t="n">
+        <v>800.9299999999999</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>800.9299999999999</v>
+      <c r="A17" s="2" t="n">
+        <v>45749</v>
       </c>
       <c r="B17" t="n">
         <v>764.244</v>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>45749</v>
+      <c r="C17" t="n">
+        <v>800.9299999999999</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>797.116</v>
+      <c r="A18" s="2" t="n">
+        <v>45750</v>
       </c>
       <c r="B18" t="n">
         <v>753.74</v>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>45750</v>
+      <c r="C18" t="n">
+        <v>797.116</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>791.395</v>
+      <c r="A19" s="2" t="n">
+        <v>45751</v>
       </c>
       <c r="B19" t="n">
         <v>730.444</v>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>45751</v>
+      <c r="C19" t="n">
+        <v>791.395</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>781.86</v>
+      <c r="A20" s="2" t="n">
+        <v>45754</v>
       </c>
       <c r="B20" t="n">
         <v>679.38</v>
       </c>
-      <c r="C20" s="2" t="n">
+      <c r="C20" t="n">
+        <v>781.86</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
         <v>45754</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>781.86</v>
       </c>
       <c r="B21" t="n">
         <v>679.38</v>
       </c>
-      <c r="C21" s="2" t="n">
+      <c r="C21" t="n">
+        <v>781.86</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
         <v>45754</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>781.86</v>
       </c>
       <c r="B22" t="n">
         <v>679.38</v>
       </c>
-      <c r="C22" s="2" t="n">
+      <c r="C22" t="n">
+        <v>781.86</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
         <v>45754</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>781.86</v>
       </c>
       <c r="B23" t="n">
         <v>679.38</v>
       </c>
-      <c r="C23" s="2" t="n">
-        <v>45754</v>
+      <c r="C23" t="n">
+        <v>781.86</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>779.953</v>
+      <c r="A24" s="2" t="n">
+        <v>45755</v>
       </c>
       <c r="B24" t="n">
         <v>690.04</v>
       </c>
-      <c r="C24" s="2" t="n">
-        <v>45755</v>
+      <c r="C24" t="n">
+        <v>779.953</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>776.14</v>
+      <c r="A25" s="2" t="n">
+        <v>45756</v>
       </c>
       <c r="B25" t="n">
         <v>673.0359999999999</v>
       </c>
-      <c r="C25" s="2" t="n">
-        <v>45756</v>
+      <c r="C25" t="n">
+        <v>776.14</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>770.419</v>
+      <c r="A26" s="2" t="n">
+        <v>45757</v>
       </c>
       <c r="B26" t="n">
         <v>697.8920000000001</v>
       </c>
-      <c r="C26" s="2" t="n">
-        <v>45757</v>
+      <c r="C26" t="n">
+        <v>770.419</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>770.419</v>
+      <c r="A27" s="2" t="n">
+        <v>45758</v>
       </c>
       <c r="B27" t="n">
         <v>692.068</v>
       </c>
-      <c r="C27" s="2" t="n">
-        <v>45758</v>
+      <c r="C27" t="n">
+        <v>770.419</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>781.86</v>
+      <c r="A28" s="2" t="n">
+        <v>45754</v>
       </c>
       <c r="B28" t="n">
         <v>679.38</v>
       </c>
-      <c r="C28" s="2" t="n">
-        <v>45754</v>
+      <c r="C28" t="n">
+        <v>781.86</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>770.419</v>
+      <c r="A29" s="2" t="n">
+        <v>45757</v>
       </c>
       <c r="B29" t="n">
         <v>697.8920000000001</v>
       </c>
-      <c r="C29" s="2" t="n">
-        <v>45757</v>
+      <c r="C29" t="n">
+        <v>770.419</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>770.419</v>
+      <c r="A30" s="2" t="n">
+        <v>45758</v>
       </c>
       <c r="B30" t="n">
         <v>692.068</v>
       </c>
-      <c r="C30" s="2" t="n">
+      <c r="C30" t="n">
+        <v>770.419</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
         <v>45758</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>770.419</v>
       </c>
       <c r="B31" t="n">
         <v>692.068</v>
       </c>
-      <c r="C31" s="3" t="n">
+      <c r="C31" t="n">
+        <v>770.419</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="n">
         <v>45758</v>
+      </c>
+      <c r="B32" t="n">
+        <v>692.068</v>
+      </c>
+      <c r="C32" t="n">
+        <v>770.419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-18 06:01
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -16,11 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -60,13 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -432,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,356 +443,120 @@
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>LNBSF00</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>MLBSO00</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45734</v>
-      </c>
-      <c r="B2" t="n">
-        <v>790.4</v>
-      </c>
-      <c r="C2" t="n">
-        <v>806.651</v>
+        <v>45728</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45733</v>
-      </c>
-      <c r="B3" t="n">
-        <v>795.08</v>
-      </c>
-      <c r="C3" t="n">
-        <v>810.465</v>
+        <v>45729</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
         <v>45730</v>
       </c>
-      <c r="B4" t="n">
-        <v>792.8440000000001</v>
-      </c>
-      <c r="C4" t="n">
-        <v>810.465</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45729</v>
-      </c>
-      <c r="B5" t="n">
-        <v>803.816</v>
-      </c>
-      <c r="C5" t="n">
-        <v>810.465</v>
+        <v>45733</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45728</v>
-      </c>
-      <c r="B6" t="n">
-        <v>802.724</v>
-      </c>
-      <c r="C6" t="n">
-        <v>810.465</v>
+        <v>45734</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
         <v>45735</v>
       </c>
-      <c r="B7" t="n">
-        <v>808.9640000000001</v>
-      </c>
-      <c r="C7" t="n">
-        <v>806.651</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
         <v>45736</v>
       </c>
-      <c r="B8" t="n">
-        <v>823.3680000000001</v>
-      </c>
-      <c r="C8" t="n">
-        <v>806.651</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
         <v>45737</v>
       </c>
-      <c r="B9" t="n">
-        <v>823.9400000000001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>806.651</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
         <v>45740</v>
       </c>
-      <c r="B10" t="n">
-        <v>788.6319999999999</v>
-      </c>
-      <c r="C10" t="n">
-        <v>806.651</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
         <v>45741</v>
       </c>
-      <c r="B11" t="n">
-        <v>785.928</v>
-      </c>
-      <c r="C11" t="n">
-        <v>806.651</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
         <v>45742</v>
       </c>
-      <c r="B12" t="n">
-        <v>773.9160000000001</v>
-      </c>
-      <c r="C12" t="n">
-        <v>806.651</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45734</v>
-      </c>
-      <c r="B13" t="n">
-        <v>790.4</v>
-      </c>
-      <c r="C13" t="n">
-        <v>806.651</v>
+        <v>45743</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45743</v>
-      </c>
-      <c r="B14" t="n">
-        <v>771.1079999999999</v>
-      </c>
-      <c r="C14" t="n">
-        <v>806.651</v>
+        <v>45744</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45744</v>
-      </c>
-      <c r="B15" t="n">
-        <v>760.188</v>
-      </c>
-      <c r="C15" t="n">
-        <v>800.9299999999999</v>
+        <v>45748</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45748</v>
-      </c>
-      <c r="B16" t="n">
-        <v>749.736</v>
-      </c>
-      <c r="C16" t="n">
-        <v>800.9299999999999</v>
+        <v>45749</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45749</v>
-      </c>
-      <c r="B17" t="n">
-        <v>764.244</v>
-      </c>
-      <c r="C17" t="n">
-        <v>800.9299999999999</v>
+        <v>45750</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45750</v>
-      </c>
-      <c r="B18" t="n">
-        <v>753.74</v>
-      </c>
-      <c r="C18" t="n">
-        <v>797.116</v>
+        <v>45751</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45751</v>
-      </c>
-      <c r="B19" t="n">
-        <v>730.444</v>
-      </c>
-      <c r="C19" t="n">
-        <v>791.395</v>
+        <v>45754</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45754</v>
-      </c>
-      <c r="B20" t="n">
-        <v>679.38</v>
-      </c>
-      <c r="C20" t="n">
-        <v>781.86</v>
+        <v>45755</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45754</v>
-      </c>
-      <c r="B21" t="n">
-        <v>679.38</v>
-      </c>
-      <c r="C21" t="n">
-        <v>781.86</v>
+        <v>45756</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45754</v>
-      </c>
-      <c r="B22" t="n">
-        <v>679.38</v>
-      </c>
-      <c r="C22" t="n">
-        <v>781.86</v>
+        <v>45757</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45754</v>
-      </c>
-      <c r="B23" t="n">
-        <v>679.38</v>
-      </c>
-      <c r="C23" t="n">
-        <v>781.86</v>
+        <v>45758</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45755</v>
-      </c>
-      <c r="B24" t="n">
-        <v>690.04</v>
-      </c>
-      <c r="C24" t="n">
-        <v>779.953</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="2" t="n">
-        <v>45756</v>
-      </c>
-      <c r="B25" t="n">
-        <v>673.0359999999999</v>
-      </c>
-      <c r="C25" t="n">
-        <v>776.14</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="n">
-        <v>45757</v>
-      </c>
-      <c r="B26" t="n">
-        <v>697.8920000000001</v>
-      </c>
-      <c r="C26" t="n">
-        <v>770.419</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="n">
-        <v>45758</v>
-      </c>
-      <c r="B27" t="n">
-        <v>692.068</v>
-      </c>
-      <c r="C27" t="n">
-        <v>770.419</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="n">
-        <v>45754</v>
-      </c>
-      <c r="B28" t="n">
-        <v>679.38</v>
-      </c>
-      <c r="C28" t="n">
-        <v>781.86</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="2" t="n">
-        <v>45757</v>
-      </c>
-      <c r="B29" t="n">
-        <v>697.8920000000001</v>
-      </c>
-      <c r="C29" t="n">
-        <v>770.419</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="n">
-        <v>45758</v>
-      </c>
-      <c r="B30" t="n">
-        <v>692.068</v>
-      </c>
-      <c r="C30" t="n">
-        <v>770.419</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="n">
-        <v>45758</v>
-      </c>
-      <c r="B31" t="n">
-        <v>692.068</v>
-      </c>
-      <c r="C31" t="n">
-        <v>770.419</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="3" t="n">
-        <v>45758</v>
-      </c>
-      <c r="B32" t="n">
-        <v>692.068</v>
-      </c>
-      <c r="C32" t="n">
-        <v>770.419</v>
+        <v>45761</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-18 06:02
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -564,6 +564,11 @@
         <v>45762</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45763</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-21 02:42
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A26"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -569,6 +569,11 @@
         <v>45763</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45764</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-21 09:21
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,136 +443,209 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>LNBSF00</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>MLBSO00</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45728</v>
+        <v>45764</v>
+      </c>
+      <c r="B2" t="n">
+        <v>753.948</v>
+      </c>
+      <c r="C2" t="n">
+        <v>758.977</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45729</v>
-      </c>
+        <v>45764</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45730</v>
-      </c>
+        <v>45763</v>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45733</v>
-      </c>
+        <v>45762</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45734</v>
-      </c>
+        <v>45761</v>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45735</v>
-      </c>
+        <v>45758</v>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45736</v>
-      </c>
+        <v>45757</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45737</v>
-      </c>
+        <v>45756</v>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45740</v>
-      </c>
+        <v>45755</v>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45741</v>
-      </c>
+        <v>45754</v>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45742</v>
-      </c>
+        <v>45751</v>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45743</v>
-      </c>
+        <v>45750</v>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45744</v>
-      </c>
+        <v>45749</v>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
         <v>45748</v>
       </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45749</v>
-      </c>
+        <v>45744</v>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45750</v>
-      </c>
+        <v>45743</v>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45751</v>
-      </c>
+        <v>45742</v>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45754</v>
-      </c>
+        <v>45741</v>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45755</v>
-      </c>
+        <v>45740</v>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45756</v>
-      </c>
+        <v>45737</v>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45757</v>
-      </c>
+        <v>45736</v>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45758</v>
-      </c>
+        <v>45735</v>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45761</v>
-      </c>
+        <v>45734</v>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45762</v>
-      </c>
+        <v>45733</v>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45763</v>
-      </c>
+        <v>45730</v>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45764</v>
-      </c>
+        <v>45729</v>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>45728</v>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-21 09:22
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -440,7 +440,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>MLBSO00</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -450,202 +450,202 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>MLBSO00</t>
+          <t>Date</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" s="2" t="n">
         <v>45764</v>
       </c>
-      <c r="B2" t="n">
-        <v>753.948</v>
-      </c>
-      <c r="C2" t="n">
-        <v>758.977</v>
-      </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45764</v>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" s="2" t="n">
+        <v>45763</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
+      <c r="A4" t="n">
+        <v>770.419</v>
+      </c>
+      <c r="B4" t="n">
+        <v>725.452</v>
+      </c>
+      <c r="C4" s="2" t="n">
         <v>45763</v>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" s="2" t="n">
         <v>45762</v>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" s="2" t="n">
         <v>45761</v>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" s="2" t="n">
         <v>45758</v>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" s="2" t="n">
         <v>45757</v>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" s="2" t="n">
         <v>45756</v>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" s="2" t="n">
         <v>45755</v>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" s="2" t="n">
         <v>45754</v>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" s="2" t="n">
         <v>45751</v>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" s="2" t="n">
         <v>45750</v>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" s="2" t="n">
         <v>45749</v>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="n">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" s="2" t="n">
         <v>45748</v>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="n">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" s="2" t="n">
         <v>45744</v>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="n">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" s="2" t="n">
         <v>45743</v>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="n">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" s="2" t="n">
         <v>45742</v>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="n">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" s="2" t="n">
         <v>45741</v>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="n">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" s="2" t="n">
         <v>45740</v>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="n">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" s="2" t="n">
         <v>45737</v>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="n">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" s="2" t="n">
         <v>45736</v>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="n">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" s="2" t="n">
         <v>45735</v>
       </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="n">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" s="2" t="n">
         <v>45734</v>
       </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="n">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" s="2" t="n">
         <v>45733</v>
       </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="n">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" s="2" t="n">
         <v>45730</v>
       </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="n">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" s="2" t="n">
         <v>45729</v>
       </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="n">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" s="2" t="n">
         <v>45728</v>
       </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-21 09:31
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,8 +462,12 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
+      <c r="A3" t="n">
+        <v>770.419</v>
+      </c>
+      <c r="B3" t="n">
+        <v>725.452</v>
+      </c>
       <c r="C3" s="2" t="n">
         <v>45763</v>
       </c>
@@ -473,177 +477,170 @@
         <v>770.419</v>
       </c>
       <c r="B4" t="n">
-        <v>725.452</v>
+        <v>717.028</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45763</v>
+        <v>45762</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr"/>
       <c r="C5" s="2" t="n">
-        <v>45762</v>
+        <v>45761</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr"/>
       <c r="C6" s="2" t="n">
-        <v>45761</v>
+        <v>45758</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr"/>
       <c r="C7" s="2" t="n">
-        <v>45758</v>
+        <v>45757</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr"/>
       <c r="C8" s="2" t="n">
-        <v>45757</v>
+        <v>45756</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr"/>
       <c r="C9" s="2" t="n">
-        <v>45756</v>
+        <v>45755</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr"/>
       <c r="C10" s="2" t="n">
-        <v>45755</v>
+        <v>45754</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr"/>
       <c r="C11" s="2" t="n">
-        <v>45754</v>
+        <v>45751</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr"/>
       <c r="C12" s="2" t="n">
-        <v>45751</v>
+        <v>45750</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr"/>
       <c r="C13" s="2" t="n">
-        <v>45750</v>
+        <v>45749</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr"/>
       <c r="C14" s="2" t="n">
-        <v>45749</v>
+        <v>45748</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr"/>
       <c r="C15" s="2" t="n">
-        <v>45748</v>
+        <v>45744</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr"/>
       <c r="C16" s="2" t="n">
-        <v>45744</v>
+        <v>45743</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr"/>
       <c r="C17" s="2" t="n">
-        <v>45743</v>
+        <v>45742</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr"/>
       <c r="C18" s="2" t="n">
-        <v>45742</v>
+        <v>45741</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr"/>
       <c r="C19" s="2" t="n">
-        <v>45741</v>
+        <v>45740</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr"/>
       <c r="C20" s="2" t="n">
-        <v>45740</v>
+        <v>45737</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr"/>
       <c r="C21" s="2" t="n">
-        <v>45737</v>
+        <v>45736</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr"/>
       <c r="C22" s="2" t="n">
-        <v>45736</v>
+        <v>45735</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr"/>
       <c r="C23" s="2" t="n">
-        <v>45735</v>
+        <v>45734</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr"/>
       <c r="C24" s="2" t="n">
-        <v>45734</v>
+        <v>45733</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr"/>
       <c r="C25" s="2" t="n">
-        <v>45733</v>
+        <v>45730</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
       <c r="B26" t="inlineStr"/>
       <c r="C26" s="2" t="n">
-        <v>45730</v>
+        <v>45729</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr"/>
       <c r="C27" s="2" t="n">
-        <v>45729</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr"/>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" s="2" t="n">
         <v>45728</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-25 02:47
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,7 +440,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MLBSO00</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -450,199 +450,210 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>MLBSO00</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" s="2" t="n">
+      <c r="A2" s="2" t="n">
+        <v>45768</v>
+      </c>
+      <c r="B2" t="n">
+        <v>758.1079999999999</v>
+      </c>
+      <c r="C2" t="n">
+        <v>755.163</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
         <v>45764</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45763</v>
+      </c>
+      <c r="B4" t="n">
+        <v>725.452</v>
+      </c>
+      <c r="C4" t="n">
         <v>770.419</v>
       </c>
-      <c r="B3" t="n">
-        <v>725.452</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>45763</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B5" t="n">
+        <v>717.028</v>
+      </c>
+      <c r="C5" t="n">
         <v>770.419</v>
       </c>
-      <c r="B4" t="n">
-        <v>717.028</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>45762</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" s="2" t="n">
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
         <v>45761</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr"/>
-      <c r="C6" s="2" t="n">
+      <c r="C6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
         <v>45758</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr"/>
-      <c r="C7" s="2" t="n">
+      <c r="C7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
         <v>45757</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr"/>
-      <c r="C8" s="2" t="n">
+      <c r="C8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
         <v>45756</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr"/>
-      <c r="C9" s="2" t="n">
+      <c r="C9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
         <v>45755</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr"/>
-      <c r="C10" s="2" t="n">
+      <c r="C10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
         <v>45754</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr"/>
-      <c r="C11" s="2" t="n">
+      <c r="C11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
         <v>45751</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr"/>
-      <c r="C12" s="2" t="n">
+      <c r="C12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
         <v>45750</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr"/>
-      <c r="C13" s="2" t="n">
+      <c r="C13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
         <v>45749</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" s="2" t="n">
+      <c r="C14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
         <v>45748</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" s="2" t="n">
+      <c r="C15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
         <v>45744</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr"/>
-      <c r="C16" s="2" t="n">
+      <c r="C16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
         <v>45743</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" s="2" t="n">
+      <c r="C17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
         <v>45742</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr"/>
-      <c r="C18" s="2" t="n">
+      <c r="C18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
         <v>45741</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr"/>
-      <c r="C19" s="2" t="n">
+      <c r="C19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
         <v>45740</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" s="2" t="n">
+      <c r="C20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
         <v>45737</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" s="2" t="n">
+      <c r="C21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
         <v>45736</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr"/>
-      <c r="C22" s="2" t="n">
+      <c r="C22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
         <v>45735</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr"/>
-      <c r="C23" s="2" t="n">
+      <c r="C23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
         <v>45734</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr"/>
-      <c r="C24" s="2" t="n">
+      <c r="C24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
         <v>45733</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr"/>
-      <c r="C25" s="2" t="n">
+      <c r="C25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
         <v>45730</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr"/>
       <c r="B26" t="inlineStr"/>
-      <c r="C26" s="2" t="n">
+      <c r="C26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
         <v>45729</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr"/>
-      <c r="C27" s="2" t="n">
+      <c r="C27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
         <v>45728</v>
       </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update FuelPrices at 2025-04-25 02:48
</commit_message>
<xml_diff>
--- a/data/fuel_prices.xlsx
+++ b/data/fuel_prices.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,10 +456,10 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45770</v>
+        <v>45771</v>
       </c>
       <c r="B2" t="n">
-        <v>722.956</v>
+        <v>700.96</v>
       </c>
       <c r="C2" t="n">
         <v>753.256</v>
@@ -467,10 +467,10 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45769</v>
+        <v>45770</v>
       </c>
       <c r="B3" t="n">
-        <v>748.228</v>
+        <v>722.956</v>
       </c>
       <c r="C3" t="n">
         <v>753.256</v>
@@ -478,39 +478,39 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45768</v>
+        <v>45769</v>
       </c>
       <c r="B4" t="n">
-        <v>758.1079999999999</v>
+        <v>748.228</v>
       </c>
       <c r="C4" t="n">
-        <v>755.163</v>
+        <v>753.256</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45764</v>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
+        <v>45768</v>
+      </c>
+      <c r="B5" t="n">
+        <v>758.1079999999999</v>
+      </c>
+      <c r="C5" t="n">
+        <v>755.163</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45763</v>
-      </c>
-      <c r="B6" t="n">
-        <v>725.452</v>
-      </c>
-      <c r="C6" t="n">
-        <v>770.419</v>
-      </c>
+        <v>45764</v>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45762</v>
+        <v>45763</v>
       </c>
       <c r="B7" t="n">
-        <v>717.028</v>
+        <v>725.452</v>
       </c>
       <c r="C7" t="n">
         <v>770.419</v>
@@ -518,164 +518,175 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
+        <v>45762</v>
+      </c>
+      <c r="B8" t="n">
+        <v>717.028</v>
+      </c>
+      <c r="C8" t="n">
+        <v>770.419</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45758</v>
+        <v>45761</v>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45757</v>
+        <v>45758</v>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45756</v>
+        <v>45757</v>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45755</v>
+        <v>45756</v>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45754</v>
+        <v>45755</v>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45751</v>
+        <v>45754</v>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45750</v>
+        <v>45751</v>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45749</v>
+        <v>45750</v>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45748</v>
+        <v>45749</v>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45744</v>
+        <v>45748</v>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45742</v>
+        <v>45743</v>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45736</v>
+        <v>45737</v>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45735</v>
+        <v>45736</v>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45734</v>
+        <v>45735</v>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45733</v>
+        <v>45734</v>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45730</v>
+        <v>45733</v>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45729</v>
+        <v>45730</v>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45728</v>
+        <v>45729</v>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45728</v>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>